<commit_message>
Adds two implemented test cases
</commit_message>
<xml_diff>
--- a/CSTPostOffice/domainMatrixPostOffice.xlsx
+++ b/CSTPostOffice/domainMatrixPostOffice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhmff\Desktop\IST\MEIC\1ano\2semestre\TVS\Projeto\CSTPostOffice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ED05B8-FA3E-4683-BEC8-AB4E7224A20D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A923AEE6-2725-46BE-BF7D-111FB691B7BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,21 +57,12 @@
     <t>Typical</t>
   </si>
   <si>
-    <t>&lt;= maxNumberOfProducts</t>
-  </si>
-  <si>
-    <t>maxNumberOfProducts</t>
-  </si>
-  <si>
     <t>&gt;= 2</t>
   </si>
   <si>
     <t>&lt;= 20</t>
   </si>
   <si>
-    <t>po.products</t>
-  </si>
-  <si>
     <t xml:space="preserve">p.price </t>
   </si>
   <si>
@@ -94,6 +85,15 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>po.getNumberOfProducts()</t>
+  </si>
+  <si>
+    <t>&lt;= po.maxNumberOfProducts</t>
+  </si>
+  <si>
+    <t>po.maxNumberOfProducts</t>
   </si>
 </sst>
 </file>
@@ -252,24 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -277,12 +259,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,6 +268,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,20 +582,20 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.21875" customWidth="1"/>
     <col min="2" max="2" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
@@ -616,10 +616,10 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="1">
         <v>1</v>
       </c>
@@ -656,22 +656,22 @@
       <c r="O2" s="1">
         <v>12</v>
       </c>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -684,19 +684,19 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -708,13 +708,13 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -723,45 +723,45 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
+        <v>16</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
+      <c r="A6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -780,13 +780,13 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
@@ -804,13 +804,13 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -848,16 +848,16 @@
       <c r="O8" s="1">
         <v>11</v>
       </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>12</v>
+      <c r="A9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -876,13 +876,13 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
@@ -900,14 +900,14 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
+      <c r="A11" s="16"/>
+      <c r="B11" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -926,13 +926,13 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
@@ -950,13 +950,13 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -988,16 +988,16 @@
         <v>15</v>
       </c>
       <c r="O13" s="1"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>16</v>
+      <c r="A14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -1016,14 +1016,14 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="10" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="1"/>
@@ -1040,16 +1040,16 @@
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1">
@@ -1084,16 +1084,16 @@
       <c r="O16" s="1">
         <v>89</v>
       </c>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>16</v>
+      <c r="A17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
@@ -1112,13 +1112,13 @@
         <v>0</v>
       </c>
       <c r="O17" s="1"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1136,16 +1136,16 @@
       <c r="O18" s="1">
         <v>-1</v>
       </c>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="10"/>
+      <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="1">
@@ -1180,58 +1180,64 @@
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
+        <v>18</v>
+      </c>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A20:C20"/>
@@ -1241,13 +1247,8 @@
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes test case 2
</commit_message>
<xml_diff>
--- a/CSTPostOffice/domainMatrixPostOffice.xlsx
+++ b/CSTPostOffice/domainMatrixPostOffice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhmff\Desktop\IST\MEIC\1ano\2semestre\TVS\Projeto\CSTPostOffice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A923AEE6-2725-46BE-BF7D-111FB691B7BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2697D1-0E41-4FC3-B0FA-FBC5C5E92BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -269,34 +269,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -582,7 +582,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,34 +592,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="1">
         <v>1</v>
       </c>
@@ -661,10 +661,10 @@
       <c r="R2" s="7"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -689,8 +689,8 @@
       <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -713,7 +713,7 @@
       <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -757,10 +757,10 @@
       <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -785,8 +785,8 @@
       <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
@@ -809,7 +809,7 @@
       <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -853,10 +853,10 @@
       <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -881,8 +881,8 @@
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
@@ -905,8 +905,8 @@
       <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -931,8 +931,8 @@
       <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
@@ -955,7 +955,7 @@
       <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -972,7 +972,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -993,10 +993,10 @@
       <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1021,8 +1021,8 @@
       <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1089,10 +1089,10 @@
       <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1117,8 +1117,8 @@
       <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1185,11 +1185,11 @@
       <c r="R19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>19</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>18</v>
@@ -1232,12 +1232,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A20:C20"/>
@@ -1247,6 +1241,12 @@
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adds test cases fixed
</commit_message>
<xml_diff>
--- a/CSTPostOffice/domainMatrixPostOffice.xlsx
+++ b/CSTPostOffice/domainMatrixPostOffice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhmff\Desktop\IST\MEIC\1ano\2semestre\TVS\Projeto\CSTPostOffice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2697D1-0E41-4FC3-B0FA-FBC5C5E92BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F50DE21-C95A-4CE6-BD41-5A4FBE35A4B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,34 +269,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -582,44 +582,44 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="1">
         <v>1</v>
       </c>
@@ -661,10 +661,10 @@
       <c r="R2" s="7"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -689,8 +689,8 @@
       <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -713,7 +713,7 @@
       <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -757,10 +757,10 @@
       <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -785,8 +785,8 @@
       <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
@@ -809,7 +809,7 @@
       <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -825,7 +825,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I8" s="1">
         <v>5</v>
@@ -853,10 +853,10 @@
       <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -881,8 +881,8 @@
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
@@ -905,8 +905,8 @@
       <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -931,8 +931,8 @@
       <c r="R11" s="7"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
@@ -955,7 +955,7 @@
       <c r="R12" s="7"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -993,10 +993,10 @@
       <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1021,8 +1021,8 @@
       <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1089,10 +1089,10 @@
       <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1117,8 +1117,8 @@
       <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
@@ -1185,11 +1185,11 @@
       <c r="R19" s="7"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="12"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>19</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>18</v>
@@ -1232,6 +1232,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A20:C20"/>
@@ -1241,12 +1247,6 @@
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adds final test cases
</commit_message>
<xml_diff>
--- a/CSTPostOffice/domainMatrixPostOffice.xlsx
+++ b/CSTPostOffice/domainMatrixPostOffice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhmff\Desktop\IST\MEIC\1ano\2semestre\TVS\Projeto\CSTPostOffice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F50DE21-C95A-4CE6-BD41-5A4FBE35A4B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DCC827-A682-43A7-BFA3-3F7D3D26DA2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,114 +140,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,44 +156,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -582,7 +451,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,34 +461,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1">
         <v>1</v>
       </c>
@@ -656,15 +525,15 @@
       <c r="O2" s="1">
         <v>12</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -684,13 +553,13 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -708,12 +577,12 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -752,15 +621,15 @@
       <c r="O5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -780,13 +649,13 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
@@ -804,12 +673,12 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -848,15 +717,15 @@
       <c r="O8" s="1">
         <v>11</v>
       </c>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -876,13 +745,13 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
@@ -900,13 +769,13 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -926,13 +795,13 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
@@ -950,12 +819,12 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -987,16 +856,18 @@
       <c r="N13" s="1">
         <v>15</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
+      <c r="O13" s="1">
+        <v>17</v>
+      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1016,13 +887,13 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1040,12 +911,12 @@
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1084,15 +955,15 @@
       <c r="O16" s="1">
         <v>89</v>
       </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1112,13 +983,13 @@
         <v>0</v>
       </c>
       <c r="O17" s="1"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1136,16 +1007,16 @@
       <c r="O18" s="1">
         <v>-1</v>
       </c>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="1">
@@ -1180,16 +1051,16 @@
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1226,18 +1097,14 @@
       <c r="O20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:O1"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="A20:C20"/>
@@ -1247,6 +1114,10 @@
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>